<commit_message>
Add Fixed XPath and Random time
</commit_message>
<xml_diff>
--- a/number_list.xlsx
+++ b/number_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\PycharmProjects\Whats_App_Message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF934C-57D0-4B93-91FB-67540EAA530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C5D6BB-2F04-46EF-BAC2-F878920D3A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1330" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A774"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -396,7 +396,9 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>79526937578</v>
+      </c>
     </row>
     <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
Fixed Account and QR
</commit_message>
<xml_diff>
--- a/number_list.xlsx
+++ b/number_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\PycharmProjects\Whats_App_Message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C5D6BB-2F04-46EF-BAC2-F878920D3A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9E0B92-4FC9-40C2-906B-9E298BD48BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="1330" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A774"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -396,9 +396,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>79526937578</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>

</xml_diff>